<commit_message>
changed 12mOhm and 39mOhm resistors
</commit_message>
<xml_diff>
--- a/Schematics/BOMs/Main BOM.xlsx
+++ b/Schematics/BOMs/Main BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basbw\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFB51E6-90AB-4643-A7F6-6ED6A63550AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C7678D-330F-44DB-9C34-E7BABB6503B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{6A6E9F8A-266D-4918-87D5-86BD9D7295F9}"/>
+    <workbookView xWindow="14655" yWindow="0" windowWidth="23850" windowHeight="20985" xr2:uid="{6A6E9F8A-266D-4918-87D5-86BD9D7295F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -356,19 +356,19 @@
     <t>MF1/4DCT52R2201F</t>
   </si>
   <si>
-    <t>603-PE1206DRM470R012</t>
-  </si>
-  <si>
-    <t>PE1206DRM470R012L</t>
-  </si>
-  <si>
     <t>YAGEO</t>
   </si>
   <si>
-    <t>603-PE1206DRM470R039</t>
-  </si>
-  <si>
-    <t>PE1206DRM470R039L</t>
+    <t>PE2512DKE070R04L</t>
+  </si>
+  <si>
+    <t>603-PE2512DKE070R04L</t>
+  </si>
+  <si>
+    <t>667-ERJ-6CWDR012V</t>
+  </si>
+  <si>
+    <t>ERJ-6CWDR012V</t>
   </si>
 </sst>
 </file>
@@ -784,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5988E4C-923E-4723-B8A6-3EF937B71B6F}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -1021,7 +1021,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="25.5">
+    <row r="7" spans="1:13">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1045,13 +1045,13 @@
         <v>26</v>
       </c>
       <c r="K7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1075,13 +1075,13 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
+        <v>106</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:13">

</xml_diff>